<commit_message>
test clients web package
</commit_message>
<xml_diff>
--- a/report_null.xlsx
+++ b/report_null.xlsx
@@ -38,25 +38,25 @@
     <t>Quantité</t>
   </si>
   <si>
-    <t>shopping with Pissarro</t>
+    <t>shopping with Ansel Adams</t>
   </si>
   <si>
-    <t>2014-01-09</t>
+    <t>2013-06-15</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Lightweight Leather Bag</t>
+    <t>Heavy Duty Concrete Shirt</t>
   </si>
   <si>
-    <t>Cous Cous</t>
+    <t>Turnips</t>
   </si>
   <si>
     <t>4.0</t>
   </si>
   <si>
-    <t>3.0</t>
+    <t>2.0</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
exclude entities/dto from code coverage
</commit_message>
<xml_diff>
--- a/report_null.xlsx
+++ b/report_null.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -38,25 +38,22 @@
     <t>Quantité</t>
   </si>
   <si>
-    <t>shopping with Ansel Adams</t>
+    <t>shopping with Kahlo</t>
   </si>
   <si>
-    <t>2013-06-15</t>
+    <t>1950-11-30</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Heavy Duty Concrete Shirt</t>
+    <t>Mediocre Wool Coat</t>
   </si>
   <si>
-    <t>Turnips</t>
+    <t>Celery Seed</t>
   </si>
   <si>
-    <t>4.0</t>
-  </si>
-  <si>
-    <t>2.0</t>
+    <t>5.0</t>
   </si>
 </sst>
 </file>
@@ -180,7 +177,7 @@
         <v>13</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add unit testing on legacy code
</commit_message>
<xml_diff>
--- a/report_null.xlsx
+++ b/report_null.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -38,22 +38,25 @@
     <t>Quantité</t>
   </si>
   <si>
-    <t>shopping with Kahlo</t>
+    <t>shopping with Degas</t>
   </si>
   <si>
-    <t>1950-11-30</t>
+    <t>1971-08-27</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Mediocre Wool Coat</t>
+    <t>Lightweight Wool Bench</t>
   </si>
   <si>
-    <t>Celery Seed</t>
+    <t>Tea</t>
   </si>
   <si>
-    <t>5.0</t>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>2.0</t>
   </si>
 </sst>
 </file>
@@ -177,7 +180,7 @@
         <v>13</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
003: add bucketController (define bucket web services)
</commit_message>
<xml_diff>
--- a/report_null.xlsx
+++ b/report_null.xlsx
@@ -38,25 +38,25 @@
     <t>Quantité</t>
   </si>
   <si>
-    <t>shopping with Degas</t>
+    <t>shopping with Escher</t>
   </si>
   <si>
-    <t>1971-08-27</t>
+    <t>1951-05-06</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Lightweight Wool Bench</t>
+    <t>Enormous Plastic Bottle</t>
   </si>
   <si>
-    <t>Tea</t>
+    <t>Mustard Seed</t>
   </si>
   <si>
     <t>4.0</t>
   </si>
   <si>
-    <t>2.0</t>
+    <t>3.0</t>
   </si>
 </sst>
 </file>

</xml_diff>